<commit_message>
plotting GSDs by Q classification
</commit_message>
<xml_diff>
--- a/data_analysis/GSD_trap_vs_WC_analysis/samples_grouped_by_Q/Q_groups_forGSD.xlsx
+++ b/data_analysis/GSD_trap_vs_WC_analysis/samples_grouped_by_Q/Q_groups_forGSD.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data_analysis\GSD_trap_vs_WC_analysis\samples_grouped_by_Q\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410925D-2BE1-41C2-9291-E33E68F6F1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7607CE-9A9B-4244-B274-018FD8338468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView minimized="1" xWindow="-20895" yWindow="2625" windowWidth="8925" windowHeight="8550" xr2:uid="{F0384620-6BCB-45FB-A616-E3A7A6BDB0EC}"/>
+    <workbookView minimized="1" xWindow="-20895" yWindow="2625" windowWidth="8925" windowHeight="8550" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring" sheetId="1" r:id="rId1"/>
@@ -357,8 +356,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -427,8 +426,8 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -447,7 +446,7 @@
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -460,10 +459,10 @@
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -485,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -494,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -780,10 +779,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:P15"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="O9" sqref="O9:Q9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +835,7 @@
         <v>0.171886328011326</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f>IF(C2&lt;$G$3,"Low Q", IF(C2&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" ref="D2:D43" si="0">IF(C2&lt;$G$3,"Low Q", IF(C2&lt;$G$4, "Mod Q", "High Q"))</f>
         <v>Low Q</v>
       </c>
       <c r="F2" t="s">
@@ -883,7 +879,7 @@
         <v>0.17858253626276399</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>IF(C3&lt;$G$3,"Low Q", IF(C3&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="F3" t="s">
@@ -925,7 +921,7 @@
         <v>0.17366943358482301</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>IF(C4&lt;$G$3,"Low Q", IF(C4&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="F4" t="s">
@@ -967,7 +963,7 @@
         <v>0.16965170896000101</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f>IF(C5&lt;$G$3,"Low Q", IF(C5&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="F5" t="s">
@@ -1012,7 +1008,7 @@
         <v>0.184383366461084</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f>IF(C6&lt;$G$3,"Low Q", IF(C6&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="G6" s="2"/>
@@ -1048,7 +1044,7 @@
         <v>0.18482722940617299</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f>IF(C7&lt;$G$3,"Low Q", IF(C7&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="F7" t="s">
@@ -1090,7 +1086,7 @@
         <v>0.17679177852632699</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f>IF(C8&lt;$G$3,"Low Q", IF(C8&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="F8" t="s">
@@ -1123,7 +1119,7 @@
         <v>0.17366943358482301</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f>IF(C9&lt;$G$3,"Low Q", IF(C9&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="H9" s="2"/>
@@ -1158,7 +1154,7 @@
         <v>0.176808528840387</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f>IF(C10&lt;$G$3,"Low Q", IF(C10&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="H10" s="2"/>
@@ -1193,7 +1189,7 @@
         <v>0.18666898145639299</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f>IF(C11&lt;$G$3,"Low Q", IF(C11&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K11" s="10">
@@ -1227,7 +1223,7 @@
         <v>0.186683051720204</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f>IF(C12&lt;$G$3,"Low Q", IF(C12&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K12" s="10">
@@ -1260,7 +1256,7 @@
         <v>0.18257120581726999</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f>IF(C13&lt;$G$3,"Low Q", IF(C13&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K13" s="10">
@@ -1293,7 +1289,7 @@
         <v>0.198135555256964</v>
       </c>
       <c r="D14" s="14" t="str">
-        <f>IF(C14&lt;$G$3,"Low Q", IF(C14&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
       <c r="K14" s="10">
@@ -1326,7 +1322,7 @@
         <v>0.202196770380911</v>
       </c>
       <c r="D15" s="14" t="str">
-        <f>IF(C15&lt;$G$3,"Low Q", IF(C15&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
       <c r="K15" s="10">
@@ -1359,7 +1355,7 @@
         <v>0.19323818890813499</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f>IF(C16&lt;$G$3,"Low Q", IF(C16&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K16" s="10">
@@ -1386,7 +1382,7 @@
         <v>0.228024805885122</v>
       </c>
       <c r="D17" s="14" t="str">
-        <f>IF(C17&lt;$G$3,"Low Q", IF(C17&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
       <c r="K17" s="10">
@@ -1410,7 +1406,7 @@
         <v>0.277136428383431</v>
       </c>
       <c r="D18" s="6" t="str">
-        <f>IF(C18&lt;$G$3,"Low Q", IF(C18&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
       <c r="K18" s="10">
@@ -1434,7 +1430,7 @@
         <v>0.26457163552462398</v>
       </c>
       <c r="D19" s="6" t="str">
-        <f>IF(C19&lt;$G$3,"Low Q", IF(C19&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
       <c r="K19" s="10">
@@ -1458,7 +1454,7 @@
         <v>0.24797493203292101</v>
       </c>
       <c r="D20" s="6" t="str">
-        <f>IF(C20&lt;$G$3,"Low Q", IF(C20&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
       <c r="K20" s="10">
@@ -1482,7 +1478,7 @@
         <v>0.184383366461084</v>
       </c>
       <c r="D21" s="9" t="str">
-        <f>IF(C21&lt;$G$3,"Low Q", IF(C21&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K21" s="10">
@@ -1506,7 +1502,7 @@
         <v>0.18482722940617299</v>
       </c>
       <c r="D22" s="9" t="str">
-        <f>IF(C22&lt;$G$3,"Low Q", IF(C22&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K22" s="10">
@@ -1530,7 +1526,7 @@
         <v>0.17679177852632699</v>
       </c>
       <c r="D23" s="9" t="str">
-        <f>IF(C23&lt;$G$3,"Low Q", IF(C23&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K23" s="10">
@@ -1554,7 +1550,7 @@
         <v>0.17278170769464399</v>
       </c>
       <c r="D24" s="9" t="str">
-        <f>IF(C24&lt;$G$3,"Low Q", IF(C24&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K24" s="10">
@@ -1578,7 +1574,7 @@
         <v>0.19405093533895701</v>
       </c>
       <c r="D25" s="9" t="str">
-        <f>IF(C25&lt;$G$3,"Low Q", IF(C25&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K25" s="10">
@@ -1602,7 +1598,7 @@
         <v>0.19159893063024599</v>
       </c>
       <c r="D26" s="9" t="str">
-        <f>IF(C26&lt;$G$3,"Low Q", IF(C26&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K26" s="10">
@@ -1626,7 +1622,7 @@
         <v>0.181738892085264</v>
       </c>
       <c r="D27" s="9" t="str">
-        <f>IF(C27&lt;$G$3,"Low Q", IF(C27&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K27" s="10">
@@ -1650,7 +1646,7 @@
         <v>0.16521002777305599</v>
       </c>
       <c r="D28" s="9" t="str">
-        <f>IF(C28&lt;$G$3,"Low Q", IF(C28&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K28" s="10">
@@ -1674,7 +1670,7 @@
         <v>0.16105877013360401</v>
       </c>
       <c r="D29" s="9" t="str">
-        <f>IF(C29&lt;$G$3,"Low Q", IF(C29&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K29" s="10">
@@ -1698,7 +1694,7 @@
         <v>0.15938753872582101</v>
       </c>
       <c r="D30" s="9" t="str">
-        <f>IF(C30&lt;$G$3,"Low Q", IF(C30&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K30" s="10">
@@ -1722,7 +1718,7 @@
         <v>0.16105877013360401</v>
       </c>
       <c r="D31" s="9" t="str">
-        <f>IF(C31&lt;$G$3,"Low Q", IF(C31&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
       <c r="K31" s="10">
@@ -1746,7 +1742,7 @@
         <v>0.17433150869914599</v>
       </c>
       <c r="D32" s="9" t="str">
-        <f>IF(C32&lt;$G$3,"Low Q", IF(C32&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1761,7 +1757,7 @@
         <v>0.18995671353775601</v>
       </c>
       <c r="D33" s="9" t="str">
-        <f>IF(C33&lt;$G$3,"Low Q", IF(C33&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1776,7 +1772,7 @@
         <v>0.18995671353775601</v>
       </c>
       <c r="D34" s="9" t="str">
-        <f>IF(C34&lt;$G$3,"Low Q", IF(C34&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1791,7 +1787,7 @@
         <v>0.15354232467829301</v>
       </c>
       <c r="D35" s="9" t="str">
-        <f>IF(C35&lt;$G$3,"Low Q", IF(C35&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1806,7 +1802,7 @@
         <v>0.169350687476575</v>
       </c>
       <c r="D36" s="9" t="str">
-        <f>IF(C36&lt;$G$3,"Low Q", IF(C36&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1821,7 +1817,7 @@
         <v>0.18666898145639299</v>
       </c>
       <c r="D37" s="9" t="str">
-        <f>IF(C37&lt;$G$3,"Low Q", IF(C37&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
     </row>
@@ -1836,7 +1832,7 @@
         <v>0.198135555256964</v>
       </c>
       <c r="D38" s="14" t="str">
-        <f>IF(C38&lt;$G$3,"Low Q", IF(C38&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
     </row>
@@ -1851,7 +1847,7 @@
         <v>0.21435307565376299</v>
       </c>
       <c r="D39" s="14" t="str">
-        <f>IF(C39&lt;$G$3,"Low Q", IF(C39&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
     </row>
@@ -1866,7 +1862,7 @@
         <v>0.277136428383431</v>
       </c>
       <c r="D40" s="6" t="str">
-        <f>IF(C40&lt;$G$3,"Low Q", IF(C40&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
     </row>
@@ -1881,7 +1877,7 @@
         <v>0.25114191513496997</v>
       </c>
       <c r="D41" s="6" t="str">
-        <f>IF(C41&lt;$G$3,"Low Q", IF(C41&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
     </row>
@@ -1896,7 +1892,7 @@
         <v>0.24797493203292101</v>
       </c>
       <c r="D42" s="6" t="str">
-        <f>IF(C42&lt;$G$3,"Low Q", IF(C42&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>High Q</v>
       </c>
     </row>
@@ -1911,7 +1907,7 @@
         <v>0.216775431899037</v>
       </c>
       <c r="D43" s="14" t="str">
-        <f>IF(C43&lt;$G$3,"Low Q", IF(C43&lt;$G$4, "Mod Q", "High Q"))</f>
+        <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
     </row>
@@ -1926,9 +1922,8 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
plots by flow categories (did not work)
</commit_message>
<xml_diff>
--- a/data_analysis/GSD_trap_vs_WC_analysis/samples_grouped_by_Q/Q_groups_forGSD.xlsx
+++ b/data_analysis/GSD_trap_vs_WC_analysis/samples_grouped_by_Q/Q_groups_forGSD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data_analysis\GSD_trap_vs_WC_analysis\samples_grouped_by_Q\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7607CE-9A9B-4244-B274-018FD8338468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF8A2AC-BEAB-44FF-B6DB-D32BFC314AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-20895" yWindow="2625" windowWidth="8925" windowHeight="8550" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="108">
   <si>
     <t>Date_Time</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>ST7-U7</t>
+  </si>
+  <si>
+    <t>RANGE</t>
+  </si>
+  <si>
+    <t>INTERVALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total q </t>
+  </si>
+  <si>
+    <t>just samples</t>
   </si>
 </sst>
 </file>
@@ -779,7 +791,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,6 +817,9 @@
       <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
       <c r="K1" s="3" t="s">
         <v>52</v>
       </c>
@@ -1192,6 +1207,9 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F11" t="s">
+        <v>106</v>
+      </c>
       <c r="K11" s="10">
         <v>45046.75</v>
       </c>
@@ -1226,6 +1244,12 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.2E-2</v>
+      </c>
       <c r="K12" s="10">
         <v>45046.958333333336</v>
       </c>
@@ -1259,6 +1283,13 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="1">
+        <f>G12+G18</f>
+        <v>0.10733333333333332</v>
+      </c>
       <c r="K13" s="10">
         <v>45047.583333333336</v>
       </c>
@@ -1292,6 +1323,13 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="1">
+        <f>G13+G18</f>
+        <v>0.20266666666666666</v>
+      </c>
       <c r="K14" s="10">
         <v>45048.416666666664</v>
       </c>
@@ -1325,6 +1363,12 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.29799999999999999</v>
+      </c>
       <c r="K15" s="10">
         <v>45034.6875</v>
       </c>
@@ -1385,6 +1429,13 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17">
+        <f>G15-G12</f>
+        <v>0.28599999999999998</v>
+      </c>
       <c r="K17" s="10">
         <v>45035.104166666664</v>
       </c>
@@ -1408,6 +1459,13 @@
       <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>High Q</v>
+      </c>
+      <c r="F18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18">
+        <f>G17/3</f>
+        <v>9.5333333333333325E-2</v>
       </c>
       <c r="K18" s="10">
         <v>45035.3125</v>
@@ -1922,7 +1980,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,6 +2005,9 @@
       <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="I1" s="3" t="s">
         <v>52</v>
       </c>
@@ -2278,6 +2339,9 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
       <c r="I10" s="10">
         <v>45151.876388888886</v>
       </c>
@@ -2311,6 +2375,12 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>2E-3</v>
+      </c>
       <c r="I11" s="10">
         <v>45151.78125</v>
       </c>
@@ -2344,6 +2414,13 @@
         <f t="shared" si="0"/>
         <v>Mod Q</v>
       </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <f>G11+G17</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
       <c r="I12" s="10">
         <v>45151.791666666664</v>
       </c>
@@ -2377,6 +2454,13 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13">
+        <f>G12+G17</f>
+        <v>6.6000000000000003E-2</v>
+      </c>
       <c r="I13" s="10">
         <v>45151.802083333336</v>
       </c>
@@ -2410,6 +2494,12 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14">
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="I14" s="10">
         <v>45151.8125</v>
       </c>
@@ -2476,6 +2566,13 @@
         <f t="shared" si="0"/>
         <v>Low Q</v>
       </c>
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16">
+        <f>G14-G11</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
       <c r="I16" s="10">
         <v>45151.833333333336</v>
       </c>
@@ -2499,6 +2596,13 @@
       <c r="D17" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Low Q</v>
+      </c>
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17">
+        <f>G16/3</f>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="I17" s="10">
         <v>45151.84375</v>

</xml_diff>